<commit_message>
Updated paramsheets and hdmix
Conversion functions are not case sensitive.
Function descriptions have been added to the paramsheet functions and the save_results function.
</commit_message>
<xml_diff>
--- a/IonExchangeModel/test/data/reg_test_input.xlsx
+++ b/IonExchangeModel/test/data/reg_test_input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhaupert\IEXpy\HSDM\JBB\to_github\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdatsov\OneDrive - Environmental Protection Agency (EPA)\Profile\Documents\GitHub\Water_Treatment_Models\IonExchangeModel\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAF7774-D52B-4664-9D53-72AE3FFEB4A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{FFAF7774-D52B-4664-9D53-72AE3FFEB4A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{8B99820C-9984-437B-91DE-F549A7384A02}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="-15630" windowWidth="21600" windowHeight="11370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="2" r:id="rId1"/>
@@ -45,79 +45,79 @@
     <t>valence</t>
   </si>
   <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>rb</t>
+  </si>
+  <si>
+    <t>nr</t>
+  </si>
+  <si>
+    <t>nz</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>meq</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>hr</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>meq/g</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>cm/s</t>
+  </si>
+  <si>
+    <t>cm2/s</t>
+  </si>
+  <si>
+    <t>flrt</t>
+  </si>
+  <si>
+    <t>diam</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>lb/ft3</t>
+  </si>
+  <si>
+    <t>gpm</t>
+  </si>
+  <si>
+    <t>Ds</t>
+  </si>
+  <si>
+    <t>kL</t>
+  </si>
+  <si>
+    <t>EBED</t>
+  </si>
+  <si>
+    <t>RHOP</t>
+  </si>
+  <si>
     <t>Qm</t>
-  </si>
-  <si>
-    <t>RHOP</t>
-  </si>
-  <si>
-    <t>EBED</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>rb</t>
-  </si>
-  <si>
-    <t>kL</t>
-  </si>
-  <si>
-    <t>nr</t>
-  </si>
-  <si>
-    <t>nz</t>
-  </si>
-  <si>
-    <t>Ds</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>units</t>
-  </si>
-  <si>
-    <t>meq</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>hr</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>meq/g</t>
-  </si>
-  <si>
-    <t>cm</t>
-  </si>
-  <si>
-    <t>cm/s</t>
-  </si>
-  <si>
-    <t>cm2/s</t>
-  </si>
-  <si>
-    <t>flrt</t>
-  </si>
-  <si>
-    <t>diam</t>
-  </si>
-  <si>
-    <t>in</t>
-  </si>
-  <si>
-    <t>lb/ft3</t>
-  </si>
-  <si>
-    <t>gpm</t>
   </si>
 </sst>
 </file>
@@ -963,48 +963,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>1.5</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>39.33</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>0.38</v>
@@ -1012,73 +1012,73 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>10.199999999999999</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>3.4500000000000003E-2</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1">
         <v>2.2000000000000001E-3</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1">
         <v>4.9999999999999998E-8</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3">
         <v>9</v>
@@ -1086,7 +1086,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <v>13</v>
@@ -1094,13 +1094,13 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1123,7 +1123,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -1135,7 +1135,7 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1152,7 +1152,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1169,7 +1169,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1186,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1203,7 +1203,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1215,7 +1215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1223,7 +1223,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>

</xml_diff>